<commit_message>
Han sido borradas ciertas referencias
</commit_message>
<xml_diff>
--- a/08 - Analysis and representation of X-CNV results/Resultados/tabla_10.xlsx
+++ b/08 - Analysis and representation of X-CNV results/Resultados/tabla_10.xlsx
@@ -86,34 +86,34 @@
     <t>DEL</t>
   </si>
   <si>
-    <t>AFA016</t>
-  </si>
-  <si>
-    <t>CAM-GFF-107</t>
-  </si>
-  <si>
-    <t>CAM-GFF-119</t>
-  </si>
-  <si>
-    <t>CAM-GFF-37</t>
-  </si>
-  <si>
-    <t>CAM-GUI-039</t>
-  </si>
-  <si>
-    <t>CAM-GUI-129</t>
-  </si>
-  <si>
-    <t>CAM-PYKL-140</t>
-  </si>
-  <si>
-    <t>CAM-PYKL-144</t>
-  </si>
-  <si>
-    <t>TK-KVBAF069</t>
-  </si>
-  <si>
-    <t>WAZ118</t>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 11</t>
+  </si>
+  <si>
+    <t>Sample 14</t>
+  </si>
+  <si>
+    <t>Sample 16</t>
+  </si>
+  <si>
+    <t>Sample 22</t>
+  </si>
+  <si>
+    <t>Sample 26</t>
+  </si>
+  <si>
+    <t>Sample 47</t>
+  </si>
+  <si>
+    <t>Sample 48</t>
+  </si>
+  <si>
+    <t>Sample 88</t>
+  </si>
+  <si>
+    <t>Sample 100</t>
   </si>
   <si>
     <t>pathogenic</t>

</xml_diff>